<commit_message>
Improve identifiers and fix typos
</commit_message>
<xml_diff>
--- a/docs/source/_files/example/BSI_MFMC_T0.xlsx
+++ b/docs/source/_files/example/BSI_MFMC_T0.xlsx
@@ -715,7 +715,7 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>GRMFMC000</t>
+          <t>EGRMFMC000</t>
         </is>
       </c>
     </row>
@@ -1334,12 +1334,12 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>XS2400040460</t>
+          <t>IXS2400040460</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>GRAK1</t>
+          <t>EGRAK1</t>
         </is>
       </c>
       <c r="C4" s="16" t="n">
@@ -23456,7 +23456,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>GRAK1</t>
+          <t>IGRAK1</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -35758,12 +35758,12 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>GRF000000001</t>
+          <t>IGRF000000001</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>I_GRMFMC000_H1</t>
+          <t>PGRMFMC000_H1</t>
         </is>
       </c>
       <c r="C4" s="16" t="n">
@@ -35803,12 +35803,12 @@
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>GRF000000001</t>
+          <t>IGRF000000001</t>
         </is>
       </c>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>I_GRMFMC000_H2</t>
+          <t>PGRMFMC000_H2</t>
         </is>
       </c>
       <c r="C5" s="16" t="n">
@@ -35848,12 +35848,12 @@
     <row r="6">
       <c r="A6" s="12" t="inlineStr">
         <is>
-          <t>GRF000000001</t>
+          <t>IGRF000000001</t>
         </is>
       </c>
       <c r="B6" s="12" t="inlineStr">
         <is>
-          <t>T_GR99999999</t>
+          <t>TGR99999999</t>
         </is>
       </c>
       <c r="C6" s="16" t="n">
@@ -37080,7 +37080,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>GR8801101230000012300302300</t>
+          <t>IGR8801101230000012300302300</t>
         </is>
       </c>
       <c r="B4" s="16" t="n">
@@ -38209,12 +38209,12 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>XS2400040460</t>
+          <t>IXS2400040460</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>GRAK1</t>
+          <t>EGRAK1</t>
         </is>
       </c>
       <c r="C4" s="16" t="n">

</xml_diff>

<commit_message>
Update files in _files
</commit_message>
<xml_diff>
--- a/docs/source/_files/example/BSI_MFMC_T0.xlsx
+++ b/docs/source/_files/example/BSI_MFMC_T0.xlsx
@@ -703,14 +703,14 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>bsi</t>
+          <t>BSI</t>
         </is>
       </c>
     </row>
     <row r="5" ht="40" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SOURCE_ORG</t>
+          <t>RA</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -722,12 +722,12 @@
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>SOURCE_PERSON</t>
+          <t>RP</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>aloumiotis@foo.gr</t>
+          <t>aloumiotis</t>
         </is>
       </c>
     </row>
@@ -4337,10 +4337,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -4357,18 +4357,19 @@
     <col width="13.5" customWidth="1" min="7" max="7"/>
     <col width="13.5" customWidth="1" min="8" max="8"/>
     <col width="13.5" customWidth="1" min="9" max="9"/>
-    <col width="10.8" customWidth="1" min="10" max="10"/>
-    <col width="9.450000000000001" customWidth="1" min="11" max="11"/>
-    <col width="13.5" customWidth="1" min="12" max="12"/>
+    <col width="13.5" customWidth="1" min="10" max="10"/>
+    <col width="10.8" customWidth="1" min="11" max="11"/>
+    <col width="9.450000000000001" customWidth="1" min="12" max="12"/>
     <col width="13.5" customWidth="1" min="13" max="13"/>
     <col width="13.5" customWidth="1" min="14" max="14"/>
     <col width="13.5" customWidth="1" min="15" max="15"/>
-    <col width="10.8" customWidth="1" min="16" max="16"/>
+    <col width="13.5" customWidth="1" min="16" max="16"/>
     <col width="10.8" customWidth="1" min="17" max="17"/>
     <col width="10.8" customWidth="1" min="18" max="18"/>
-    <col width="9.450000000000001" customWidth="1" min="19" max="19"/>
-    <col width="13.5" customWidth="1" min="20" max="20"/>
+    <col width="10.8" customWidth="1" min="19" max="19"/>
+    <col width="9.450000000000001" customWidth="1" min="20" max="20"/>
     <col width="13.5" customWidth="1" min="21" max="21"/>
+    <col width="13.5" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="60" customHeight="1">
@@ -4378,23 +4379,23 @@
         </is>
       </c>
       <c r="B1" s="7" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="C1" s="7" t="n"/>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>MEASURES</t>
         </is>
       </c>
-      <c r="E1" s="7" t="n"/>
       <c r="F1" s="7" t="n"/>
       <c r="G1" s="7" t="n"/>
       <c r="H1" s="7" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="10" t="inlineStr">
+      <c r="I1" s="7" t="n"/>
+      <c r="J1" s="8" t="n"/>
+      <c r="K1" s="10" t="inlineStr">
         <is>
           <t>ATTRS</t>
         </is>
       </c>
-      <c r="K1" s="7" t="n"/>
       <c r="L1" s="7" t="n"/>
       <c r="M1" s="7" t="n"/>
       <c r="N1" s="7" t="n"/>
@@ -4404,7 +4405,8 @@
       <c r="R1" s="7" t="n"/>
       <c r="S1" s="7" t="n"/>
       <c r="T1" s="7" t="n"/>
-      <c r="U1" s="8" t="n"/>
+      <c r="U1" s="7" t="n"/>
+      <c r="V1" s="8" t="n"/>
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" s="11" t="inlineStr">
@@ -4413,53 +4415,54 @@
         </is>
       </c>
       <c r="B2" s="7" t="n"/>
-      <c r="C2" s="8" t="n"/>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="C2" s="7" t="n"/>
+      <c r="D2" s="8" t="n"/>
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>MEASURES</t>
         </is>
       </c>
-      <c r="E2" s="7" t="n"/>
       <c r="F2" s="7" t="n"/>
       <c r="G2" s="7" t="n"/>
       <c r="H2" s="7" t="n"/>
-      <c r="I2" s="8" t="n"/>
-      <c r="J2" s="10" t="inlineStr">
+      <c r="I2" s="7" t="n"/>
+      <c r="J2" s="8" t="n"/>
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>STCK</t>
         </is>
       </c>
-      <c r="K2" s="8" t="n"/>
-      <c r="L2" s="10" t="inlineStr">
+      <c r="L2" s="8" t="n"/>
+      <c r="M2" s="10" t="inlineStr">
         <is>
           <t>EUR_STCK</t>
         </is>
       </c>
-      <c r="M2" s="8" t="n"/>
-      <c r="N2" s="10" t="inlineStr">
+      <c r="N2" s="8" t="n"/>
+      <c r="O2" s="10" t="inlineStr">
         <is>
           <t>TRNSCTNS</t>
         </is>
       </c>
-      <c r="O2" s="8" t="n"/>
-      <c r="P2" s="10" t="inlineStr">
+      <c r="P2" s="8" t="n"/>
+      <c r="Q2" s="10" t="inlineStr">
         <is>
           <t>ACCRLS</t>
         </is>
       </c>
-      <c r="Q2" s="8" t="n"/>
-      <c r="R2" s="10" t="inlineStr">
+      <c r="R2" s="8" t="n"/>
+      <c r="S2" s="10" t="inlineStr">
         <is>
           <t>ARRRS</t>
         </is>
       </c>
-      <c r="S2" s="8" t="n"/>
-      <c r="T2" s="10" t="inlineStr">
+      <c r="T2" s="8" t="n"/>
+      <c r="U2" s="10" t="inlineStr">
         <is>
           <t>WRT_OFFS</t>
         </is>
       </c>
-      <c r="U2" s="8" t="n"/>
+      <c r="V2" s="8" t="n"/>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="11" t="inlineStr">
@@ -4469,100 +4472,105 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
           <t>DT</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
           <t>FRQNCY</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
         <is>
           <t>STCK</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="F3" s="9" t="inlineStr">
         <is>
           <t>EUR_STCK</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="G3" s="9" t="inlineStr">
         <is>
           <t>TRNSCTNS</t>
         </is>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t>ACCRLS</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
         <is>
           <t>ARRRS</t>
         </is>
       </c>
-      <c r="I3" s="9" t="inlineStr">
+      <c r="J3" s="9" t="inlineStr">
         <is>
           <t>WRT_OFFS</t>
         </is>
       </c>
-      <c r="J3" s="10" t="inlineStr">
+      <c r="K3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="K3" s="10" t="inlineStr">
+      <c r="L3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="L3" s="10" t="inlineStr">
+      <c r="M3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="M3" s="10" t="inlineStr">
+      <c r="N3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="N3" s="10" t="inlineStr">
+      <c r="O3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="O3" s="10" t="inlineStr">
+      <c r="P3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="P3" s="10" t="inlineStr">
+      <c r="Q3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="Q3" s="10" t="inlineStr">
+      <c r="R3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="R3" s="10" t="inlineStr">
+      <c r="S3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="S3" s="10" t="inlineStr">
+      <c r="T3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="T3" s="10" t="inlineStr">
+      <c r="U3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="U3" s="10" t="inlineStr">
+      <c r="V3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
@@ -4572,13 +4580,13 @@
       <c r="A4" s="12" t="inlineStr"/>
       <c r="B4" s="12" t="inlineStr"/>
       <c r="C4" s="12" t="inlineStr"/>
-      <c r="D4" s="13" t="inlineStr"/>
+      <c r="D4" s="12" t="inlineStr"/>
       <c r="E4" s="13" t="inlineStr"/>
       <c r="F4" s="13" t="inlineStr"/>
       <c r="G4" s="13" t="inlineStr"/>
       <c r="H4" s="13" t="inlineStr"/>
       <c r="I4" s="13" t="inlineStr"/>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="13" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr"/>
       <c r="L4" s="14" t="inlineStr"/>
       <c r="M4" s="14" t="inlineStr"/>
@@ -4590,18 +4598,19 @@
       <c r="S4" s="14" t="inlineStr"/>
       <c r="T4" s="14" t="inlineStr"/>
       <c r="U4" s="14" t="inlineStr"/>
+      <c r="V4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="12" t="n"/>
       <c r="B5" s="12" t="n"/>
       <c r="C5" s="12" t="n"/>
-      <c r="D5" s="13" t="n"/>
+      <c r="D5" s="12" t="n"/>
       <c r="E5" s="13" t="n"/>
       <c r="F5" s="13" t="n"/>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="13" t="n"/>
       <c r="I5" s="13" t="n"/>
-      <c r="J5" s="14" t="n"/>
+      <c r="J5" s="13" t="n"/>
       <c r="K5" s="14" t="n"/>
       <c r="L5" s="14" t="n"/>
       <c r="M5" s="14" t="n"/>
@@ -4613,18 +4622,19 @@
       <c r="S5" s="14" t="n"/>
       <c r="T5" s="14" t="n"/>
       <c r="U5" s="14" t="n"/>
+      <c r="V5" s="14" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="12" t="n"/>
       <c r="B6" s="12" t="n"/>
       <c r="C6" s="12" t="n"/>
-      <c r="D6" s="13" t="n"/>
+      <c r="D6" s="12" t="n"/>
       <c r="E6" s="13" t="n"/>
       <c r="F6" s="13" t="n"/>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="13" t="n"/>
       <c r="I6" s="13" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="J6" s="13" t="n"/>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n"/>
       <c r="M6" s="14" t="n"/>
@@ -4636,18 +4646,19 @@
       <c r="S6" s="14" t="n"/>
       <c r="T6" s="14" t="n"/>
       <c r="U6" s="14" t="n"/>
+      <c r="V6" s="14" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="n"/>
       <c r="B7" s="12" t="n"/>
       <c r="C7" s="12" t="n"/>
-      <c r="D7" s="13" t="n"/>
+      <c r="D7" s="12" t="n"/>
       <c r="E7" s="13" t="n"/>
       <c r="F7" s="13" t="n"/>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="13" t="n"/>
       <c r="I7" s="13" t="n"/>
-      <c r="J7" s="14" t="n"/>
+      <c r="J7" s="13" t="n"/>
       <c r="K7" s="14" t="n"/>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n"/>
@@ -4659,18 +4670,19 @@
       <c r="S7" s="14" t="n"/>
       <c r="T7" s="14" t="n"/>
       <c r="U7" s="14" t="n"/>
+      <c r="V7" s="14" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="12" t="n"/>
       <c r="B8" s="12" t="n"/>
       <c r="C8" s="12" t="n"/>
-      <c r="D8" s="13" t="n"/>
+      <c r="D8" s="12" t="n"/>
       <c r="E8" s="13" t="n"/>
       <c r="F8" s="13" t="n"/>
       <c r="G8" s="13" t="n"/>
       <c r="H8" s="13" t="n"/>
       <c r="I8" s="13" t="n"/>
-      <c r="J8" s="14" t="n"/>
+      <c r="J8" s="13" t="n"/>
       <c r="K8" s="14" t="n"/>
       <c r="L8" s="14" t="n"/>
       <c r="M8" s="14" t="n"/>
@@ -4682,18 +4694,19 @@
       <c r="S8" s="14" t="n"/>
       <c r="T8" s="14" t="n"/>
       <c r="U8" s="14" t="n"/>
+      <c r="V8" s="14" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="12" t="n"/>
       <c r="B9" s="12" t="n"/>
       <c r="C9" s="12" t="n"/>
-      <c r="D9" s="13" t="n"/>
+      <c r="D9" s="12" t="n"/>
       <c r="E9" s="13" t="n"/>
       <c r="F9" s="13" t="n"/>
       <c r="G9" s="13" t="n"/>
       <c r="H9" s="13" t="n"/>
       <c r="I9" s="13" t="n"/>
-      <c r="J9" s="14" t="n"/>
+      <c r="J9" s="13" t="n"/>
       <c r="K9" s="14" t="n"/>
       <c r="L9" s="14" t="n"/>
       <c r="M9" s="14" t="n"/>
@@ -4705,18 +4718,19 @@
       <c r="S9" s="14" t="n"/>
       <c r="T9" s="14" t="n"/>
       <c r="U9" s="14" t="n"/>
+      <c r="V9" s="14" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="12" t="n"/>
       <c r="B10" s="12" t="n"/>
       <c r="C10" s="12" t="n"/>
-      <c r="D10" s="13" t="n"/>
+      <c r="D10" s="12" t="n"/>
       <c r="E10" s="13" t="n"/>
       <c r="F10" s="13" t="n"/>
       <c r="G10" s="13" t="n"/>
       <c r="H10" s="13" t="n"/>
       <c r="I10" s="13" t="n"/>
-      <c r="J10" s="14" t="n"/>
+      <c r="J10" s="13" t="n"/>
       <c r="K10" s="14" t="n"/>
       <c r="L10" s="14" t="n"/>
       <c r="M10" s="14" t="n"/>
@@ -4728,18 +4742,19 @@
       <c r="S10" s="14" t="n"/>
       <c r="T10" s="14" t="n"/>
       <c r="U10" s="14" t="n"/>
+      <c r="V10" s="14" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="12" t="n"/>
       <c r="B11" s="12" t="n"/>
       <c r="C11" s="12" t="n"/>
-      <c r="D11" s="13" t="n"/>
+      <c r="D11" s="12" t="n"/>
       <c r="E11" s="13" t="n"/>
       <c r="F11" s="13" t="n"/>
       <c r="G11" s="13" t="n"/>
       <c r="H11" s="13" t="n"/>
       <c r="I11" s="13" t="n"/>
-      <c r="J11" s="14" t="n"/>
+      <c r="J11" s="13" t="n"/>
       <c r="K11" s="14" t="n"/>
       <c r="L11" s="14" t="n"/>
       <c r="M11" s="14" t="n"/>
@@ -4751,18 +4766,19 @@
       <c r="S11" s="14" t="n"/>
       <c r="T11" s="14" t="n"/>
       <c r="U11" s="14" t="n"/>
+      <c r="V11" s="14" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="n"/>
       <c r="B12" s="12" t="n"/>
       <c r="C12" s="12" t="n"/>
-      <c r="D12" s="13" t="n"/>
+      <c r="D12" s="12" t="n"/>
       <c r="E12" s="13" t="n"/>
       <c r="F12" s="13" t="n"/>
       <c r="G12" s="13" t="n"/>
       <c r="H12" s="13" t="n"/>
       <c r="I12" s="13" t="n"/>
-      <c r="J12" s="14" t="n"/>
+      <c r="J12" s="13" t="n"/>
       <c r="K12" s="14" t="n"/>
       <c r="L12" s="14" t="n"/>
       <c r="M12" s="14" t="n"/>
@@ -4774,18 +4790,19 @@
       <c r="S12" s="14" t="n"/>
       <c r="T12" s="14" t="n"/>
       <c r="U12" s="14" t="n"/>
+      <c r="V12" s="14" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="12" t="n"/>
       <c r="B13" s="12" t="n"/>
       <c r="C13" s="12" t="n"/>
-      <c r="D13" s="13" t="n"/>
+      <c r="D13" s="12" t="n"/>
       <c r="E13" s="13" t="n"/>
       <c r="F13" s="13" t="n"/>
       <c r="G13" s="13" t="n"/>
       <c r="H13" s="13" t="n"/>
       <c r="I13" s="13" t="n"/>
-      <c r="J13" s="14" t="n"/>
+      <c r="J13" s="13" t="n"/>
       <c r="K13" s="14" t="n"/>
       <c r="L13" s="14" t="n"/>
       <c r="M13" s="14" t="n"/>
@@ -4797,18 +4814,19 @@
       <c r="S13" s="14" t="n"/>
       <c r="T13" s="14" t="n"/>
       <c r="U13" s="14" t="n"/>
+      <c r="V13" s="14" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="12" t="n"/>
       <c r="B14" s="12" t="n"/>
       <c r="C14" s="12" t="n"/>
-      <c r="D14" s="13" t="n"/>
+      <c r="D14" s="12" t="n"/>
       <c r="E14" s="13" t="n"/>
       <c r="F14" s="13" t="n"/>
       <c r="G14" s="13" t="n"/>
       <c r="H14" s="13" t="n"/>
       <c r="I14" s="13" t="n"/>
-      <c r="J14" s="14" t="n"/>
+      <c r="J14" s="13" t="n"/>
       <c r="K14" s="14" t="n"/>
       <c r="L14" s="14" t="n"/>
       <c r="M14" s="14" t="n"/>
@@ -4820,18 +4838,19 @@
       <c r="S14" s="14" t="n"/>
       <c r="T14" s="14" t="n"/>
       <c r="U14" s="14" t="n"/>
+      <c r="V14" s="14" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="n"/>
       <c r="B15" s="12" t="n"/>
       <c r="C15" s="12" t="n"/>
-      <c r="D15" s="13" t="n"/>
+      <c r="D15" s="12" t="n"/>
       <c r="E15" s="13" t="n"/>
       <c r="F15" s="13" t="n"/>
       <c r="G15" s="13" t="n"/>
       <c r="H15" s="13" t="n"/>
       <c r="I15" s="13" t="n"/>
-      <c r="J15" s="14" t="n"/>
+      <c r="J15" s="13" t="n"/>
       <c r="K15" s="14" t="n"/>
       <c r="L15" s="14" t="n"/>
       <c r="M15" s="14" t="n"/>
@@ -4843,18 +4862,19 @@
       <c r="S15" s="14" t="n"/>
       <c r="T15" s="14" t="n"/>
       <c r="U15" s="14" t="n"/>
+      <c r="V15" s="14" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="12" t="n"/>
       <c r="B16" s="12" t="n"/>
       <c r="C16" s="12" t="n"/>
-      <c r="D16" s="13" t="n"/>
+      <c r="D16" s="12" t="n"/>
       <c r="E16" s="13" t="n"/>
       <c r="F16" s="13" t="n"/>
       <c r="G16" s="13" t="n"/>
       <c r="H16" s="13" t="n"/>
       <c r="I16" s="13" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="J16" s="13" t="n"/>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n"/>
       <c r="M16" s="14" t="n"/>
@@ -4866,18 +4886,19 @@
       <c r="S16" s="14" t="n"/>
       <c r="T16" s="14" t="n"/>
       <c r="U16" s="14" t="n"/>
+      <c r="V16" s="14" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="12" t="n"/>
       <c r="B17" s="12" t="n"/>
       <c r="C17" s="12" t="n"/>
-      <c r="D17" s="13" t="n"/>
+      <c r="D17" s="12" t="n"/>
       <c r="E17" s="13" t="n"/>
       <c r="F17" s="13" t="n"/>
       <c r="G17" s="13" t="n"/>
       <c r="H17" s="13" t="n"/>
       <c r="I17" s="13" t="n"/>
-      <c r="J17" s="14" t="n"/>
+      <c r="J17" s="13" t="n"/>
       <c r="K17" s="14" t="n"/>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n"/>
@@ -4889,18 +4910,19 @@
       <c r="S17" s="14" t="n"/>
       <c r="T17" s="14" t="n"/>
       <c r="U17" s="14" t="n"/>
+      <c r="V17" s="14" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="12" t="n"/>
       <c r="B18" s="12" t="n"/>
       <c r="C18" s="12" t="n"/>
-      <c r="D18" s="13" t="n"/>
+      <c r="D18" s="12" t="n"/>
       <c r="E18" s="13" t="n"/>
       <c r="F18" s="13" t="n"/>
       <c r="G18" s="13" t="n"/>
       <c r="H18" s="13" t="n"/>
       <c r="I18" s="13" t="n"/>
-      <c r="J18" s="14" t="n"/>
+      <c r="J18" s="13" t="n"/>
       <c r="K18" s="14" t="n"/>
       <c r="L18" s="14" t="n"/>
       <c r="M18" s="14" t="n"/>
@@ -4912,18 +4934,19 @@
       <c r="S18" s="14" t="n"/>
       <c r="T18" s="14" t="n"/>
       <c r="U18" s="14" t="n"/>
+      <c r="V18" s="14" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="12" t="n"/>
       <c r="B19" s="12" t="n"/>
       <c r="C19" s="12" t="n"/>
-      <c r="D19" s="13" t="n"/>
+      <c r="D19" s="12" t="n"/>
       <c r="E19" s="13" t="n"/>
       <c r="F19" s="13" t="n"/>
       <c r="G19" s="13" t="n"/>
       <c r="H19" s="13" t="n"/>
       <c r="I19" s="13" t="n"/>
-      <c r="J19" s="14" t="n"/>
+      <c r="J19" s="13" t="n"/>
       <c r="K19" s="14" t="n"/>
       <c r="L19" s="14" t="n"/>
       <c r="M19" s="14" t="n"/>
@@ -4935,18 +4958,19 @@
       <c r="S19" s="14" t="n"/>
       <c r="T19" s="14" t="n"/>
       <c r="U19" s="14" t="n"/>
+      <c r="V19" s="14" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="12" t="n"/>
       <c r="B20" s="12" t="n"/>
       <c r="C20" s="12" t="n"/>
-      <c r="D20" s="13" t="n"/>
+      <c r="D20" s="12" t="n"/>
       <c r="E20" s="13" t="n"/>
       <c r="F20" s="13" t="n"/>
       <c r="G20" s="13" t="n"/>
       <c r="H20" s="13" t="n"/>
       <c r="I20" s="13" t="n"/>
-      <c r="J20" s="14" t="n"/>
+      <c r="J20" s="13" t="n"/>
       <c r="K20" s="14" t="n"/>
       <c r="L20" s="14" t="n"/>
       <c r="M20" s="14" t="n"/>
@@ -4958,18 +4982,19 @@
       <c r="S20" s="14" t="n"/>
       <c r="T20" s="14" t="n"/>
       <c r="U20" s="14" t="n"/>
+      <c r="V20" s="14" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="12" t="n"/>
       <c r="B21" s="12" t="n"/>
       <c r="C21" s="12" t="n"/>
-      <c r="D21" s="13" t="n"/>
+      <c r="D21" s="12" t="n"/>
       <c r="E21" s="13" t="n"/>
       <c r="F21" s="13" t="n"/>
       <c r="G21" s="13" t="n"/>
       <c r="H21" s="13" t="n"/>
       <c r="I21" s="13" t="n"/>
-      <c r="J21" s="14" t="n"/>
+      <c r="J21" s="13" t="n"/>
       <c r="K21" s="14" t="n"/>
       <c r="L21" s="14" t="n"/>
       <c r="M21" s="14" t="n"/>
@@ -4981,18 +5006,19 @@
       <c r="S21" s="14" t="n"/>
       <c r="T21" s="14" t="n"/>
       <c r="U21" s="14" t="n"/>
+      <c r="V21" s="14" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="12" t="n"/>
       <c r="B22" s="12" t="n"/>
       <c r="C22" s="12" t="n"/>
-      <c r="D22" s="13" t="n"/>
+      <c r="D22" s="12" t="n"/>
       <c r="E22" s="13" t="n"/>
       <c r="F22" s="13" t="n"/>
       <c r="G22" s="13" t="n"/>
       <c r="H22" s="13" t="n"/>
       <c r="I22" s="13" t="n"/>
-      <c r="J22" s="14" t="n"/>
+      <c r="J22" s="13" t="n"/>
       <c r="K22" s="14" t="n"/>
       <c r="L22" s="14" t="n"/>
       <c r="M22" s="14" t="n"/>
@@ -5004,18 +5030,19 @@
       <c r="S22" s="14" t="n"/>
       <c r="T22" s="14" t="n"/>
       <c r="U22" s="14" t="n"/>
+      <c r="V22" s="14" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="12" t="n"/>
       <c r="B23" s="12" t="n"/>
       <c r="C23" s="12" t="n"/>
-      <c r="D23" s="13" t="n"/>
+      <c r="D23" s="12" t="n"/>
       <c r="E23" s="13" t="n"/>
       <c r="F23" s="13" t="n"/>
       <c r="G23" s="13" t="n"/>
       <c r="H23" s="13" t="n"/>
       <c r="I23" s="13" t="n"/>
-      <c r="J23" s="14" t="n"/>
+      <c r="J23" s="13" t="n"/>
       <c r="K23" s="14" t="n"/>
       <c r="L23" s="14" t="n"/>
       <c r="M23" s="14" t="n"/>
@@ -5027,59 +5054,60 @@
       <c r="S23" s="14" t="n"/>
       <c r="T23" s="14" t="n"/>
       <c r="U23" s="14" t="n"/>
+      <c r="V23" s="14" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J1:U1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <dataValidations count="13">
-    <dataValidation sqref="C4:C20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="D4:D20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$A$1:$A$35</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'RESIDENTIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -5390,10 +5418,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -5410,18 +5438,19 @@
     <col width="13.5" customWidth="1" min="7" max="7"/>
     <col width="13.5" customWidth="1" min="8" max="8"/>
     <col width="13.5" customWidth="1" min="9" max="9"/>
-    <col width="10.8" customWidth="1" min="10" max="10"/>
-    <col width="9.450000000000001" customWidth="1" min="11" max="11"/>
-    <col width="13.5" customWidth="1" min="12" max="12"/>
+    <col width="13.5" customWidth="1" min="10" max="10"/>
+    <col width="10.8" customWidth="1" min="11" max="11"/>
+    <col width="9.450000000000001" customWidth="1" min="12" max="12"/>
     <col width="13.5" customWidth="1" min="13" max="13"/>
     <col width="13.5" customWidth="1" min="14" max="14"/>
     <col width="13.5" customWidth="1" min="15" max="15"/>
-    <col width="10.8" customWidth="1" min="16" max="16"/>
+    <col width="13.5" customWidth="1" min="16" max="16"/>
     <col width="10.8" customWidth="1" min="17" max="17"/>
     <col width="10.8" customWidth="1" min="18" max="18"/>
-    <col width="9.450000000000001" customWidth="1" min="19" max="19"/>
-    <col width="13.5" customWidth="1" min="20" max="20"/>
+    <col width="10.8" customWidth="1" min="19" max="19"/>
+    <col width="9.450000000000001" customWidth="1" min="20" max="20"/>
     <col width="13.5" customWidth="1" min="21" max="21"/>
+    <col width="13.5" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="60" customHeight="1">
@@ -5431,23 +5460,23 @@
         </is>
       </c>
       <c r="B1" s="7" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="C1" s="7" t="n"/>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>MEASURES</t>
         </is>
       </c>
-      <c r="E1" s="7" t="n"/>
       <c r="F1" s="7" t="n"/>
       <c r="G1" s="7" t="n"/>
       <c r="H1" s="7" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="10" t="inlineStr">
+      <c r="I1" s="7" t="n"/>
+      <c r="J1" s="8" t="n"/>
+      <c r="K1" s="10" t="inlineStr">
         <is>
           <t>ATTRS</t>
         </is>
       </c>
-      <c r="K1" s="7" t="n"/>
       <c r="L1" s="7" t="n"/>
       <c r="M1" s="7" t="n"/>
       <c r="N1" s="7" t="n"/>
@@ -5457,7 +5486,8 @@
       <c r="R1" s="7" t="n"/>
       <c r="S1" s="7" t="n"/>
       <c r="T1" s="7" t="n"/>
-      <c r="U1" s="8" t="n"/>
+      <c r="U1" s="7" t="n"/>
+      <c r="V1" s="8" t="n"/>
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" s="11" t="inlineStr">
@@ -5466,53 +5496,54 @@
         </is>
       </c>
       <c r="B2" s="7" t="n"/>
-      <c r="C2" s="8" t="n"/>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="C2" s="7" t="n"/>
+      <c r="D2" s="8" t="n"/>
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>MEASURES</t>
         </is>
       </c>
-      <c r="E2" s="7" t="n"/>
       <c r="F2" s="7" t="n"/>
       <c r="G2" s="7" t="n"/>
       <c r="H2" s="7" t="n"/>
-      <c r="I2" s="8" t="n"/>
-      <c r="J2" s="10" t="inlineStr">
+      <c r="I2" s="7" t="n"/>
+      <c r="J2" s="8" t="n"/>
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>STCK</t>
         </is>
       </c>
-      <c r="K2" s="8" t="n"/>
-      <c r="L2" s="10" t="inlineStr">
+      <c r="L2" s="8" t="n"/>
+      <c r="M2" s="10" t="inlineStr">
         <is>
           <t>EUR_STCK</t>
         </is>
       </c>
-      <c r="M2" s="8" t="n"/>
-      <c r="N2" s="10" t="inlineStr">
+      <c r="N2" s="8" t="n"/>
+      <c r="O2" s="10" t="inlineStr">
         <is>
           <t>TRNSCTNS</t>
         </is>
       </c>
-      <c r="O2" s="8" t="n"/>
-      <c r="P2" s="10" t="inlineStr">
+      <c r="P2" s="8" t="n"/>
+      <c r="Q2" s="10" t="inlineStr">
         <is>
           <t>ACCRLS</t>
         </is>
       </c>
-      <c r="Q2" s="8" t="n"/>
-      <c r="R2" s="10" t="inlineStr">
+      <c r="R2" s="8" t="n"/>
+      <c r="S2" s="10" t="inlineStr">
         <is>
           <t>ARRRS</t>
         </is>
       </c>
-      <c r="S2" s="8" t="n"/>
-      <c r="T2" s="10" t="inlineStr">
+      <c r="T2" s="8" t="n"/>
+      <c r="U2" s="10" t="inlineStr">
         <is>
           <t>WRT_OFFS</t>
         </is>
       </c>
-      <c r="U2" s="8" t="n"/>
+      <c r="V2" s="8" t="n"/>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" s="11" t="inlineStr">
@@ -5522,100 +5553,105 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
           <t>DT</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
           <t>FRQNCY</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
         <is>
           <t>STCK</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="F3" s="9" t="inlineStr">
         <is>
           <t>EUR_STCK</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="G3" s="9" t="inlineStr">
         <is>
           <t>TRNSCTNS</t>
         </is>
       </c>
-      <c r="G3" s="9" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t>ACCRLS</t>
         </is>
       </c>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
         <is>
           <t>ARRRS</t>
         </is>
       </c>
-      <c r="I3" s="9" t="inlineStr">
+      <c r="J3" s="9" t="inlineStr">
         <is>
           <t>WRT_OFFS</t>
         </is>
       </c>
-      <c r="J3" s="10" t="inlineStr">
+      <c r="K3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="K3" s="10" t="inlineStr">
+      <c r="L3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="L3" s="10" t="inlineStr">
+      <c r="M3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="M3" s="10" t="inlineStr">
+      <c r="N3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="N3" s="10" t="inlineStr">
+      <c r="O3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="O3" s="10" t="inlineStr">
+      <c r="P3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="P3" s="10" t="inlineStr">
+      <c r="Q3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="Q3" s="10" t="inlineStr">
+      <c r="R3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="R3" s="10" t="inlineStr">
+      <c r="S3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="S3" s="10" t="inlineStr">
+      <c r="T3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
       </c>
-      <c r="T3" s="10" t="inlineStr">
+      <c r="U3" s="10" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="U3" s="10" t="inlineStr">
+      <c r="V3" s="10" t="inlineStr">
         <is>
           <t>CONF</t>
         </is>
@@ -5625,13 +5661,13 @@
       <c r="A4" s="12" t="inlineStr"/>
       <c r="B4" s="12" t="inlineStr"/>
       <c r="C4" s="12" t="inlineStr"/>
-      <c r="D4" s="13" t="inlineStr"/>
+      <c r="D4" s="12" t="inlineStr"/>
       <c r="E4" s="13" t="inlineStr"/>
       <c r="F4" s="13" t="inlineStr"/>
       <c r="G4" s="13" t="inlineStr"/>
       <c r="H4" s="13" t="inlineStr"/>
       <c r="I4" s="13" t="inlineStr"/>
-      <c r="J4" s="14" t="inlineStr"/>
+      <c r="J4" s="13" t="inlineStr"/>
       <c r="K4" s="14" t="inlineStr"/>
       <c r="L4" s="14" t="inlineStr"/>
       <c r="M4" s="14" t="inlineStr"/>
@@ -5643,18 +5679,19 @@
       <c r="S4" s="14" t="inlineStr"/>
       <c r="T4" s="14" t="inlineStr"/>
       <c r="U4" s="14" t="inlineStr"/>
+      <c r="V4" s="14" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="12" t="n"/>
       <c r="B5" s="12" t="n"/>
       <c r="C5" s="12" t="n"/>
-      <c r="D5" s="13" t="n"/>
+      <c r="D5" s="12" t="n"/>
       <c r="E5" s="13" t="n"/>
       <c r="F5" s="13" t="n"/>
       <c r="G5" s="13" t="n"/>
       <c r="H5" s="13" t="n"/>
       <c r="I5" s="13" t="n"/>
-      <c r="J5" s="14" t="n"/>
+      <c r="J5" s="13" t="n"/>
       <c r="K5" s="14" t="n"/>
       <c r="L5" s="14" t="n"/>
       <c r="M5" s="14" t="n"/>
@@ -5666,18 +5703,19 @@
       <c r="S5" s="14" t="n"/>
       <c r="T5" s="14" t="n"/>
       <c r="U5" s="14" t="n"/>
+      <c r="V5" s="14" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="12" t="n"/>
       <c r="B6" s="12" t="n"/>
       <c r="C6" s="12" t="n"/>
-      <c r="D6" s="13" t="n"/>
+      <c r="D6" s="12" t="n"/>
       <c r="E6" s="13" t="n"/>
       <c r="F6" s="13" t="n"/>
       <c r="G6" s="13" t="n"/>
       <c r="H6" s="13" t="n"/>
       <c r="I6" s="13" t="n"/>
-      <c r="J6" s="14" t="n"/>
+      <c r="J6" s="13" t="n"/>
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n"/>
       <c r="M6" s="14" t="n"/>
@@ -5689,18 +5727,19 @@
       <c r="S6" s="14" t="n"/>
       <c r="T6" s="14" t="n"/>
       <c r="U6" s="14" t="n"/>
+      <c r="V6" s="14" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="12" t="n"/>
       <c r="B7" s="12" t="n"/>
       <c r="C7" s="12" t="n"/>
-      <c r="D7" s="13" t="n"/>
+      <c r="D7" s="12" t="n"/>
       <c r="E7" s="13" t="n"/>
       <c r="F7" s="13" t="n"/>
       <c r="G7" s="13" t="n"/>
       <c r="H7" s="13" t="n"/>
       <c r="I7" s="13" t="n"/>
-      <c r="J7" s="14" t="n"/>
+      <c r="J7" s="13" t="n"/>
       <c r="K7" s="14" t="n"/>
       <c r="L7" s="14" t="n"/>
       <c r="M7" s="14" t="n"/>
@@ -5712,18 +5751,19 @@
       <c r="S7" s="14" t="n"/>
       <c r="T7" s="14" t="n"/>
       <c r="U7" s="14" t="n"/>
+      <c r="V7" s="14" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="12" t="n"/>
       <c r="B8" s="12" t="n"/>
       <c r="C8" s="12" t="n"/>
-      <c r="D8" s="13" t="n"/>
+      <c r="D8" s="12" t="n"/>
       <c r="E8" s="13" t="n"/>
       <c r="F8" s="13" t="n"/>
       <c r="G8" s="13" t="n"/>
       <c r="H8" s="13" t="n"/>
       <c r="I8" s="13" t="n"/>
-      <c r="J8" s="14" t="n"/>
+      <c r="J8" s="13" t="n"/>
       <c r="K8" s="14" t="n"/>
       <c r="L8" s="14" t="n"/>
       <c r="M8" s="14" t="n"/>
@@ -5735,18 +5775,19 @@
       <c r="S8" s="14" t="n"/>
       <c r="T8" s="14" t="n"/>
       <c r="U8" s="14" t="n"/>
+      <c r="V8" s="14" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="12" t="n"/>
       <c r="B9" s="12" t="n"/>
       <c r="C9" s="12" t="n"/>
-      <c r="D9" s="13" t="n"/>
+      <c r="D9" s="12" t="n"/>
       <c r="E9" s="13" t="n"/>
       <c r="F9" s="13" t="n"/>
       <c r="G9" s="13" t="n"/>
       <c r="H9" s="13" t="n"/>
       <c r="I9" s="13" t="n"/>
-      <c r="J9" s="14" t="n"/>
+      <c r="J9" s="13" t="n"/>
       <c r="K9" s="14" t="n"/>
       <c r="L9" s="14" t="n"/>
       <c r="M9" s="14" t="n"/>
@@ -5758,18 +5799,19 @@
       <c r="S9" s="14" t="n"/>
       <c r="T9" s="14" t="n"/>
       <c r="U9" s="14" t="n"/>
+      <c r="V9" s="14" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="12" t="n"/>
       <c r="B10" s="12" t="n"/>
       <c r="C10" s="12" t="n"/>
-      <c r="D10" s="13" t="n"/>
+      <c r="D10" s="12" t="n"/>
       <c r="E10" s="13" t="n"/>
       <c r="F10" s="13" t="n"/>
       <c r="G10" s="13" t="n"/>
       <c r="H10" s="13" t="n"/>
       <c r="I10" s="13" t="n"/>
-      <c r="J10" s="14" t="n"/>
+      <c r="J10" s="13" t="n"/>
       <c r="K10" s="14" t="n"/>
       <c r="L10" s="14" t="n"/>
       <c r="M10" s="14" t="n"/>
@@ -5781,18 +5823,19 @@
       <c r="S10" s="14" t="n"/>
       <c r="T10" s="14" t="n"/>
       <c r="U10" s="14" t="n"/>
+      <c r="V10" s="14" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="12" t="n"/>
       <c r="B11" s="12" t="n"/>
       <c r="C11" s="12" t="n"/>
-      <c r="D11" s="13" t="n"/>
+      <c r="D11" s="12" t="n"/>
       <c r="E11" s="13" t="n"/>
       <c r="F11" s="13" t="n"/>
       <c r="G11" s="13" t="n"/>
       <c r="H11" s="13" t="n"/>
       <c r="I11" s="13" t="n"/>
-      <c r="J11" s="14" t="n"/>
+      <c r="J11" s="13" t="n"/>
       <c r="K11" s="14" t="n"/>
       <c r="L11" s="14" t="n"/>
       <c r="M11" s="14" t="n"/>
@@ -5804,18 +5847,19 @@
       <c r="S11" s="14" t="n"/>
       <c r="T11" s="14" t="n"/>
       <c r="U11" s="14" t="n"/>
+      <c r="V11" s="14" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="n"/>
       <c r="B12" s="12" t="n"/>
       <c r="C12" s="12" t="n"/>
-      <c r="D12" s="13" t="n"/>
+      <c r="D12" s="12" t="n"/>
       <c r="E12" s="13" t="n"/>
       <c r="F12" s="13" t="n"/>
       <c r="G12" s="13" t="n"/>
       <c r="H12" s="13" t="n"/>
       <c r="I12" s="13" t="n"/>
-      <c r="J12" s="14" t="n"/>
+      <c r="J12" s="13" t="n"/>
       <c r="K12" s="14" t="n"/>
       <c r="L12" s="14" t="n"/>
       <c r="M12" s="14" t="n"/>
@@ -5827,18 +5871,19 @@
       <c r="S12" s="14" t="n"/>
       <c r="T12" s="14" t="n"/>
       <c r="U12" s="14" t="n"/>
+      <c r="V12" s="14" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="12" t="n"/>
       <c r="B13" s="12" t="n"/>
       <c r="C13" s="12" t="n"/>
-      <c r="D13" s="13" t="n"/>
+      <c r="D13" s="12" t="n"/>
       <c r="E13" s="13" t="n"/>
       <c r="F13" s="13" t="n"/>
       <c r="G13" s="13" t="n"/>
       <c r="H13" s="13" t="n"/>
       <c r="I13" s="13" t="n"/>
-      <c r="J13" s="14" t="n"/>
+      <c r="J13" s="13" t="n"/>
       <c r="K13" s="14" t="n"/>
       <c r="L13" s="14" t="n"/>
       <c r="M13" s="14" t="n"/>
@@ -5850,18 +5895,19 @@
       <c r="S13" s="14" t="n"/>
       <c r="T13" s="14" t="n"/>
       <c r="U13" s="14" t="n"/>
+      <c r="V13" s="14" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="12" t="n"/>
       <c r="B14" s="12" t="n"/>
       <c r="C14" s="12" t="n"/>
-      <c r="D14" s="13" t="n"/>
+      <c r="D14" s="12" t="n"/>
       <c r="E14" s="13" t="n"/>
       <c r="F14" s="13" t="n"/>
       <c r="G14" s="13" t="n"/>
       <c r="H14" s="13" t="n"/>
       <c r="I14" s="13" t="n"/>
-      <c r="J14" s="14" t="n"/>
+      <c r="J14" s="13" t="n"/>
       <c r="K14" s="14" t="n"/>
       <c r="L14" s="14" t="n"/>
       <c r="M14" s="14" t="n"/>
@@ -5873,18 +5919,19 @@
       <c r="S14" s="14" t="n"/>
       <c r="T14" s="14" t="n"/>
       <c r="U14" s="14" t="n"/>
+      <c r="V14" s="14" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="n"/>
       <c r="B15" s="12" t="n"/>
       <c r="C15" s="12" t="n"/>
-      <c r="D15" s="13" t="n"/>
+      <c r="D15" s="12" t="n"/>
       <c r="E15" s="13" t="n"/>
       <c r="F15" s="13" t="n"/>
       <c r="G15" s="13" t="n"/>
       <c r="H15" s="13" t="n"/>
       <c r="I15" s="13" t="n"/>
-      <c r="J15" s="14" t="n"/>
+      <c r="J15" s="13" t="n"/>
       <c r="K15" s="14" t="n"/>
       <c r="L15" s="14" t="n"/>
       <c r="M15" s="14" t="n"/>
@@ -5896,18 +5943,19 @@
       <c r="S15" s="14" t="n"/>
       <c r="T15" s="14" t="n"/>
       <c r="U15" s="14" t="n"/>
+      <c r="V15" s="14" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="12" t="n"/>
       <c r="B16" s="12" t="n"/>
       <c r="C16" s="12" t="n"/>
-      <c r="D16" s="13" t="n"/>
+      <c r="D16" s="12" t="n"/>
       <c r="E16" s="13" t="n"/>
       <c r="F16" s="13" t="n"/>
       <c r="G16" s="13" t="n"/>
       <c r="H16" s="13" t="n"/>
       <c r="I16" s="13" t="n"/>
-      <c r="J16" s="14" t="n"/>
+      <c r="J16" s="13" t="n"/>
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n"/>
       <c r="M16" s="14" t="n"/>
@@ -5919,18 +5967,19 @@
       <c r="S16" s="14" t="n"/>
       <c r="T16" s="14" t="n"/>
       <c r="U16" s="14" t="n"/>
+      <c r="V16" s="14" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="12" t="n"/>
       <c r="B17" s="12" t="n"/>
       <c r="C17" s="12" t="n"/>
-      <c r="D17" s="13" t="n"/>
+      <c r="D17" s="12" t="n"/>
       <c r="E17" s="13" t="n"/>
       <c r="F17" s="13" t="n"/>
       <c r="G17" s="13" t="n"/>
       <c r="H17" s="13" t="n"/>
       <c r="I17" s="13" t="n"/>
-      <c r="J17" s="14" t="n"/>
+      <c r="J17" s="13" t="n"/>
       <c r="K17" s="14" t="n"/>
       <c r="L17" s="14" t="n"/>
       <c r="M17" s="14" t="n"/>
@@ -5942,18 +5991,19 @@
       <c r="S17" s="14" t="n"/>
       <c r="T17" s="14" t="n"/>
       <c r="U17" s="14" t="n"/>
+      <c r="V17" s="14" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="12" t="n"/>
       <c r="B18" s="12" t="n"/>
       <c r="C18" s="12" t="n"/>
-      <c r="D18" s="13" t="n"/>
+      <c r="D18" s="12" t="n"/>
       <c r="E18" s="13" t="n"/>
       <c r="F18" s="13" t="n"/>
       <c r="G18" s="13" t="n"/>
       <c r="H18" s="13" t="n"/>
       <c r="I18" s="13" t="n"/>
-      <c r="J18" s="14" t="n"/>
+      <c r="J18" s="13" t="n"/>
       <c r="K18" s="14" t="n"/>
       <c r="L18" s="14" t="n"/>
       <c r="M18" s="14" t="n"/>
@@ -5965,18 +6015,19 @@
       <c r="S18" s="14" t="n"/>
       <c r="T18" s="14" t="n"/>
       <c r="U18" s="14" t="n"/>
+      <c r="V18" s="14" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="12" t="n"/>
       <c r="B19" s="12" t="n"/>
       <c r="C19" s="12" t="n"/>
-      <c r="D19" s="13" t="n"/>
+      <c r="D19" s="12" t="n"/>
       <c r="E19" s="13" t="n"/>
       <c r="F19" s="13" t="n"/>
       <c r="G19" s="13" t="n"/>
       <c r="H19" s="13" t="n"/>
       <c r="I19" s="13" t="n"/>
-      <c r="J19" s="14" t="n"/>
+      <c r="J19" s="13" t="n"/>
       <c r="K19" s="14" t="n"/>
       <c r="L19" s="14" t="n"/>
       <c r="M19" s="14" t="n"/>
@@ -5988,18 +6039,19 @@
       <c r="S19" s="14" t="n"/>
       <c r="T19" s="14" t="n"/>
       <c r="U19" s="14" t="n"/>
+      <c r="V19" s="14" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="12" t="n"/>
       <c r="B20" s="12" t="n"/>
       <c r="C20" s="12" t="n"/>
-      <c r="D20" s="13" t="n"/>
+      <c r="D20" s="12" t="n"/>
       <c r="E20" s="13" t="n"/>
       <c r="F20" s="13" t="n"/>
       <c r="G20" s="13" t="n"/>
       <c r="H20" s="13" t="n"/>
       <c r="I20" s="13" t="n"/>
-      <c r="J20" s="14" t="n"/>
+      <c r="J20" s="13" t="n"/>
       <c r="K20" s="14" t="n"/>
       <c r="L20" s="14" t="n"/>
       <c r="M20" s="14" t="n"/>
@@ -6011,18 +6063,19 @@
       <c r="S20" s="14" t="n"/>
       <c r="T20" s="14" t="n"/>
       <c r="U20" s="14" t="n"/>
+      <c r="V20" s="14" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="12" t="n"/>
       <c r="B21" s="12" t="n"/>
       <c r="C21" s="12" t="n"/>
-      <c r="D21" s="13" t="n"/>
+      <c r="D21" s="12" t="n"/>
       <c r="E21" s="13" t="n"/>
       <c r="F21" s="13" t="n"/>
       <c r="G21" s="13" t="n"/>
       <c r="H21" s="13" t="n"/>
       <c r="I21" s="13" t="n"/>
-      <c r="J21" s="14" t="n"/>
+      <c r="J21" s="13" t="n"/>
       <c r="K21" s="14" t="n"/>
       <c r="L21" s="14" t="n"/>
       <c r="M21" s="14" t="n"/>
@@ -6034,18 +6087,19 @@
       <c r="S21" s="14" t="n"/>
       <c r="T21" s="14" t="n"/>
       <c r="U21" s="14" t="n"/>
+      <c r="V21" s="14" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="12" t="n"/>
       <c r="B22" s="12" t="n"/>
       <c r="C22" s="12" t="n"/>
-      <c r="D22" s="13" t="n"/>
+      <c r="D22" s="12" t="n"/>
       <c r="E22" s="13" t="n"/>
       <c r="F22" s="13" t="n"/>
       <c r="G22" s="13" t="n"/>
       <c r="H22" s="13" t="n"/>
       <c r="I22" s="13" t="n"/>
-      <c r="J22" s="14" t="n"/>
+      <c r="J22" s="13" t="n"/>
       <c r="K22" s="14" t="n"/>
       <c r="L22" s="14" t="n"/>
       <c r="M22" s="14" t="n"/>
@@ -6057,18 +6111,19 @@
       <c r="S22" s="14" t="n"/>
       <c r="T22" s="14" t="n"/>
       <c r="U22" s="14" t="n"/>
+      <c r="V22" s="14" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="12" t="n"/>
       <c r="B23" s="12" t="n"/>
       <c r="C23" s="12" t="n"/>
-      <c r="D23" s="13" t="n"/>
+      <c r="D23" s="12" t="n"/>
       <c r="E23" s="13" t="n"/>
       <c r="F23" s="13" t="n"/>
       <c r="G23" s="13" t="n"/>
       <c r="H23" s="13" t="n"/>
       <c r="I23" s="13" t="n"/>
-      <c r="J23" s="14" t="n"/>
+      <c r="J23" s="13" t="n"/>
       <c r="K23" s="14" t="n"/>
       <c r="L23" s="14" t="n"/>
       <c r="M23" s="14" t="n"/>
@@ -6080,59 +6135,60 @@
       <c r="S23" s="14" t="n"/>
       <c r="T23" s="14" t="n"/>
       <c r="U23" s="14" t="n"/>
+      <c r="V23" s="14" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J1:U1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <dataValidations count="13">
-    <dataValidation sqref="C4:C20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="D4:D20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$A$1:$A$35</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
-    <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
     </dataValidation>
-    <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'COMMERCIAL_RE_'!$C$1:$C$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -23456,7 +23512,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>IGRAK1</t>
+          <t>EGRAK1</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">

</xml_diff>